<commit_message>
Actualizacion de Casos de prueba
</commit_message>
<xml_diff>
--- a/Proyectos/Activos/Viaticos_q/3. Ejecución/3.3 Pruebas Internas/Viaticos_q_casos_de_prueba.xlsx
+++ b/Proyectos/Activos/Viaticos_q/3. Ejecución/3.3 Pruebas Internas/Viaticos_q_casos_de_prueba.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\IWM\Repositorio IWM\Proyectos\Activos\Viaticos_q\3. Ejecución\3.3 Pruebas internas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\Documents\cabina_press\Proyectos\Activos\Viaticos_q\3. Ejecución\3.3 Pruebas Internas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
   <si>
     <t>Pasos</t>
   </si>
@@ -216,6 +216,24 @@
   </si>
   <si>
     <t>"Viaticos_q_plan_pruebas"</t>
+  </si>
+  <si>
+    <t>CU06</t>
+  </si>
+  <si>
+    <t>8. Edicion de Gastos y Viaticos</t>
+  </si>
+  <si>
+    <t>Tras generar un viatico o Gasto se debe de poder editar el estado de la misma para cambiarlo a reportado o bien no reportado</t>
+  </si>
+  <si>
+    <t>Tener Viaticos y Gastos registrados</t>
+  </si>
+  <si>
+    <t>1. click en link reportar. O bien                          1 click en editar.                                                       2 . Click en reportar.                                                3. Click en guardar</t>
+  </si>
+  <si>
+    <t>Debe desaparecer el viatico/Gasto de la vista principal y aparecer en resumen de gastos o viaticos como reportado</t>
   </si>
 </sst>
 </file>
@@ -464,10 +482,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -483,6 +497,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -797,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,11 +834,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
     </row>
@@ -828,10 +846,10 @@
       <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="17"/>
+      <c r="D3" s="23"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
@@ -850,10 +868,10 @@
       <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="17"/>
+      <c r="D5" s="23"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
     </row>
@@ -861,10 +879,10 @@
       <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="23"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
     </row>
@@ -898,7 +916,7 @@
       <c r="E10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="17" t="s">
         <v>0</v>
       </c>
       <c r="G10" s="11" t="s">
@@ -920,316 +938,328 @@
       <c r="M10" s="8"/>
     </row>
     <row r="11" spans="2:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21" t="s">
+      <c r="G11" s="18"/>
+      <c r="H11" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
     </row>
     <row r="12" spans="2:13" ht="315" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="21" t="s">
+      <c r="G12" s="18"/>
+      <c r="H12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
     </row>
     <row r="13" spans="2:13" ht="240" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="21" t="s">
+      <c r="G13" s="18"/>
+      <c r="H13" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
     </row>
     <row r="14" spans="2:13" ht="150" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="21" t="s">
+      <c r="G14" s="18"/>
+      <c r="H14" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
     </row>
     <row r="15" spans="2:13" ht="210" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="21" t="s">
+      <c r="G15" s="18"/>
+      <c r="H15" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="2:13" ht="195" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="21" t="s">
+      <c r="G16" s="18"/>
+      <c r="H16" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
     </row>
     <row r="17" spans="2:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="21" t="s">
+      <c r="G17" s="18"/>
+      <c r="H17" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B18" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="18"/>
+      <c r="H18" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="22"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="22"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
@@ -1269,12 +1299,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>